<commit_message>
updated fields in add contacts test case
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B33F418-EDE3-4582-8733-6E18EF22F53A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B8CBCA-133E-4277-BC73-D20A57D8255C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>title</t>
   </si>
@@ -61,9 +61,6 @@
     <t>MRF</t>
   </si>
   <si>
-    <t>MRS.</t>
-  </si>
-  <si>
     <t>Mithali</t>
   </si>
   <si>
@@ -107,6 +104,66 @@
   </si>
   <si>
     <t>sachin2124563</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Crickter</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>Womens Cricket</t>
+  </si>
+  <si>
+    <t>Surgeon</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -442,15 +499,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +526,26 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -477,8 +558,26 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2">
+        <v>11111</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -491,23 +590,60 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3">
+        <v>22222</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <v>33333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -515,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309976B7-D42A-4B2F-AA38-58A2E3AB0FAF}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -532,7 +668,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -541,45 +677,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases for add deals page
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B8CBCA-133E-4277-BC73-D20A57D8255C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE15007A-0609-4EB1-9963-AFFDE062983E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>title</t>
   </si>
@@ -164,6 +164,93 @@
   </si>
   <si>
     <t>phone</t>
+  </si>
+  <si>
+    <t>primarycontact</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>commission</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>descrption</t>
+  </si>
+  <si>
+    <t>nextStep</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>deals title - 1</t>
+  </si>
+  <si>
+    <t>Flipkart company</t>
+  </si>
+  <si>
+    <t>bansal - contact</t>
+  </si>
+  <si>
+    <t>test identifier</t>
+  </si>
+  <si>
+    <t>tagOne, tagTwo, tagThree</t>
+  </si>
+  <si>
+    <t>test desc -- added by salesperson</t>
+  </si>
+  <si>
+    <t>waiting for answer from client</t>
+  </si>
+  <si>
+    <t>Test Product</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Word of Mouth</t>
+  </si>
+  <si>
+    <t>deals title - 2</t>
+  </si>
+  <si>
+    <t>Amazon Ccompany</t>
+  </si>
+  <si>
+    <t>John - Contact</t>
+  </si>
+  <si>
+    <t>Test - 2</t>
+  </si>
+  <si>
+    <t>tagFour, tagFive</t>
+  </si>
+  <si>
+    <t>test desc -- added by salesperson (amazon)</t>
+  </si>
+  <si>
+    <t>amazon - next step</t>
   </si>
 </sst>
 </file>
@@ -501,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -732,12 +819,162 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73F32D-B0D6-4212-BB6D-11E7061AFE47}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>8000</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated validations in add deals test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE15007A-0609-4EB1-9963-AFFDE062983E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E13BFA-FFF4-438C-8B2B-3CA55726F70E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>title</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>amazon - next step</t>
+  </si>
+  <si>
+    <t>predictedCloseDate</t>
+  </si>
+  <si>
+    <t>actualCloseDate</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -301,10 +313,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -819,10 +834,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73F32D-B0D6-4212-BB6D-11E7061AFE47}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +845,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
@@ -840,9 +855,11 @@
     <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +872,7 @@
       <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -885,8 +902,14 @@
       <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -899,8 +922,8 @@
       <c r="D2">
         <v>5000</v>
       </c>
-      <c r="E2">
-        <v>80</v>
+      <c r="E2" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="F2">
         <v>20</v>
@@ -929,8 +952,14 @@
       <c r="N2" t="s">
         <v>68</v>
       </c>
+      <c r="O2" s="3">
+        <v>43432</v>
+      </c>
+      <c r="P2" s="3">
+        <v>43434</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -943,8 +972,8 @@
       <c r="D3">
         <v>8000</v>
       </c>
-      <c r="E3">
-        <v>60</v>
+      <c r="E3" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -972,6 +1001,12 @@
       </c>
       <c r="N3" t="s">
         <v>68</v>
+      </c>
+      <c r="O3" s="3">
+        <v>43429</v>
+      </c>
+      <c r="P3" s="3">
+        <v>43430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases for add new tasks
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E13BFA-FFF4-438C-8B2B-3CA55726F70E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3472C75-CD1E-4AE0-AAFD-586FCAE09B23}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
   <si>
     <t>title</t>
   </si>
@@ -263,6 +263,105 @@
   </si>
   <si>
     <t>60</t>
+  </si>
+  <si>
+    <t>autoExtend</t>
+  </si>
+  <si>
+    <t>completion</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>ownerAssignedTo</t>
+  </si>
+  <si>
+    <t>keyContact</t>
+  </si>
+  <si>
+    <t>Test Title - Task 1</t>
+  </si>
+  <si>
+    <t>Test Title - Task 2</t>
+  </si>
+  <si>
+    <t>Extend deadline by 14 days</t>
+  </si>
+  <si>
+    <t>Extend deadline by 30 days</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Test deal -1</t>
+  </si>
+  <si>
+    <t>Test deal -2</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>Test case-1</t>
+  </si>
+  <si>
+    <t>Test case-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test tags -1 </t>
+  </si>
+  <si>
+    <t>Test tags -12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test desc -1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test desc -2 </t>
+  </si>
+  <si>
+    <t>Tejas niturkar</t>
+  </si>
+  <si>
+    <t>Test contact - 1</t>
+  </si>
+  <si>
+    <t>Test contact - 2</t>
+  </si>
+  <si>
+    <t>test identifier - 1</t>
+  </si>
+  <si>
+    <t>test identifier - 2</t>
+  </si>
+  <si>
+    <t>keyCompany</t>
+  </si>
+  <si>
+    <t>Test company - 1</t>
+  </si>
+  <si>
+    <t>Test company - 2</t>
   </si>
 </sst>
 </file>
@@ -836,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73F32D-B0D6-4212-BB6D-11E7061AFE47}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -1016,14 +1115,161 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E321868-2C7A-4B92-87D9-253F6B7BEAE4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="5">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="5">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding  test case for add documents
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3472C75-CD1E-4AE0-AAFD-586FCAE09B23}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B6BD25-CCAF-470F-ACC5-C3F8ABD5ABFE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="signUp" sheetId="4" r:id="rId2"/>
     <sheet name="deals" sheetId="2" r:id="rId3"/>
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
+    <sheet name="documents" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
   <si>
     <t>title</t>
   </si>
@@ -362,6 +363,27 @@
   </si>
   <si>
     <t>Test company - 2</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>Title - 1</t>
+  </si>
+  <si>
+    <t>Title - 2</t>
+  </si>
+  <si>
+    <t>Desc - 1</t>
+  </si>
+  <si>
+    <t>Desc - 2</t>
+  </si>
+  <si>
+    <t>Version -3</t>
+  </si>
+  <si>
+    <t>Version -4</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E321868-2C7A-4B92-87D9-253F6B7BEAE4}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1272,4 +1294,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F062E3-F25E-48D6-83F7-759D432EAE82}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding test case for add new company
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B6BD25-CCAF-470F-ACC5-C3F8ABD5ABFE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0515926-BE8D-4610-9528-65BD83502E01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="deals" sheetId="2" r:id="rId3"/>
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
     <sheet name="documents" sheetId="5" r:id="rId5"/>
+    <sheet name="company" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
   <si>
     <t>title</t>
   </si>
@@ -384,6 +385,177 @@
   </si>
   <si>
     <t>Version -4</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>AnnualRevenue</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>VAT/TaxNumber</t>
+  </si>
+  <si>
+    <t>AddressTitle</t>
+  </si>
+  <si>
+    <t>DefaultAddress</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tags </t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>ParentCompany</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>E-Commerce</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>test identifier -1</t>
+  </si>
+  <si>
+    <t>Vat-1</t>
+  </si>
+  <si>
+    <t>Vat-2</t>
+  </si>
+  <si>
+    <t>Main Office</t>
+  </si>
+  <si>
+    <t>Branch office</t>
+  </si>
+  <si>
+    <t>Add -1, Add-2, Add-3, Add-4</t>
+  </si>
+  <si>
+    <t>Add -7, Add-8, Add-9, Add-10</t>
+  </si>
+  <si>
+    <t>san diego</t>
+  </si>
+  <si>
+    <t>los angeles</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Tag 1</t>
+  </si>
+  <si>
+    <t>Tag 2</t>
+  </si>
+  <si>
+    <t>Test desc 1</t>
+  </si>
+  <si>
+    <t>Test desc 2</t>
+  </si>
+  <si>
+    <t>www.amazon.com1</t>
+  </si>
+  <si>
+    <t>www.microsoft.com1</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test@tes1.com</t>
+  </si>
+  <si>
+    <t>symbol -1</t>
+  </si>
+  <si>
+    <t>symbol -2</t>
+  </si>
+  <si>
+    <t>parent one</t>
+  </si>
+  <si>
+    <t>parent two</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F062E3-F25E-48D6-83F7-759D432EAE82}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1347,4 +1519,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD8986-2BA9-4E7F-9617-5EE27F2C0EA3}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W1" t="s">
+        <v>141</v>
+      </c>
+      <c r="X1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N2" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2">
+        <v>121212</v>
+      </c>
+      <c r="P2" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2">
+        <v>1125658911</v>
+      </c>
+      <c r="T2">
+        <v>798645132</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W2" t="s">
+        <v>173</v>
+      </c>
+      <c r="X2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3">
+        <v>9000000</v>
+      </c>
+      <c r="D3">
+        <v>8000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3">
+        <v>323232</v>
+      </c>
+      <c r="P3" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>166</v>
+      </c>
+      <c r="R3" t="s">
+        <v>168</v>
+      </c>
+      <c r="S3">
+        <v>9883465555</v>
+      </c>
+      <c r="T3">
+        <v>364665132</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="W3" t="s">
+        <v>174</v>
+      </c>
+      <c r="X3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{32315973-D160-45E6-ACB0-7A2AF4611A25}"/>
+    <hyperlink ref="U3" r:id="rId2" xr:uid="{185DCDB4-8E37-4E9E-895D-97774E7A878F}"/>
+    <hyperlink ref="V2" r:id="rId3" xr:uid="{1208D0CB-9F0E-4867-8E62-BED7B6C6F4C5}"/>
+    <hyperlink ref="V3" r:id="rId4" xr:uid="{BC13FE6F-CAE0-4349-BB29-52B9C9638897}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated test cases according to new channges
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0515926-BE8D-4610-9528-65BD83502E01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05BFA28-FF1C-46BD-9790-B4E22C9E1DFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="175">
   <si>
     <t>title</t>
   </si>
@@ -192,9 +192,6 @@
     <t>nextStep</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>waiting for answer from client</t>
   </si>
   <si>
-    <t>Test Product</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -342,9 +336,6 @@
     <t xml:space="preserve">Test desc -2 </t>
   </si>
   <si>
-    <t>Tejas niturkar</t>
-  </si>
-  <si>
     <t>Test contact - 1</t>
   </si>
   <si>
@@ -556,6 +547,9 @@
   </si>
   <si>
     <t>parent two</t>
+  </si>
+  <si>
+    <t>Pradumna Arts</t>
   </si>
 </sst>
 </file>
@@ -1127,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73F32D-B0D6-4212-BB6D-11E7061AFE47}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,15 +1138,14 @@
     <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.7109375" customWidth="1"/>
     <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1193,112 +1186,103 @@
         <v>57</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
       </c>
       <c r="D2">
         <v>5000</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2">
         <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>63</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
         <v>65</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>66</v>
       </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" s="3">
+        <v>43432</v>
+      </c>
+      <c r="O2" s="3">
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="N2" t="s">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="3">
-        <v>43432</v>
-      </c>
-      <c r="P2" s="3">
-        <v>43434</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
       </c>
       <c r="D3">
         <v>8000</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
         <v>72</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>73</v>
       </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
         <v>66</v>
       </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N3" t="s">
-        <v>68</v>
+      <c r="N3" s="3">
+        <v>43429</v>
       </c>
       <c r="O3" s="3">
-        <v>43429</v>
-      </c>
-      <c r="P3" s="3">
         <v>43430</v>
       </c>
     </row>
@@ -1311,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E321868-2C7A-4B92-87D9-253F6B7BEAE4}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1309,7 @@
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
@@ -1336,40 +1320,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
         <v>52</v>
       </c>
       <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" t="s">
-        <v>86</v>
-      </c>
       <c r="M1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N1" t="s">
         <v>51</v>
@@ -1377,90 +1361,90 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
       </c>
       <c r="D2" s="5">
         <v>80</v>
       </c>
       <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
       <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
         <v>99</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>101</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
         <v>103</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" t="s">
         <v>105</v>
-      </c>
-      <c r="L2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" t="s">
-        <v>111</v>
-      </c>
-      <c r="N2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="5">
         <v>90</v>
       </c>
       <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>95</v>
       </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
       <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
         <v>100</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>102</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" t="s">
         <v>104</v>
       </c>
-      <c r="K3" t="s">
-        <v>105</v>
-      </c>
-      <c r="L3" t="s">
-        <v>107</v>
-      </c>
       <c r="M3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1488,32 +1472,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD8986-2BA9-4E7F-9617-5EE27F2C0EA3}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
@@ -1550,84 +1534,84 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>125</v>
       </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>131</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>132</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>133</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>134</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>135</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>136</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>137</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>138</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>139</v>
-      </c>
-      <c r="V1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W1" t="s">
-        <v>141</v>
-      </c>
-      <c r="X1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C2">
         <v>100000</v>
@@ -1639,43 +1623,43 @@
         <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" t="s">
         <v>152</v>
       </c>
-      <c r="J2" t="s">
-        <v>153</v>
-      </c>
-      <c r="K2" t="s">
-        <v>155</v>
-      </c>
       <c r="L2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O2">
         <v>121212</v>
       </c>
       <c r="P2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Q2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="R2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="S2">
         <v>1125658911</v>
@@ -1684,24 +1668,24 @@
         <v>798645132</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="W2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="X2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C3">
         <v>9000000</v>
@@ -1710,46 +1694,46 @@
         <v>8000</v>
       </c>
       <c r="E3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" t="s">
         <v>147</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" t="s">
         <v>149</v>
       </c>
-      <c r="G3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>151</v>
       </c>
-      <c r="I3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J3" t="s">
-        <v>154</v>
-      </c>
       <c r="K3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O3">
         <v>323232</v>
       </c>
       <c r="P3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="R3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S3">
         <v>9883465555</v>
@@ -1758,16 +1742,16 @@
         <v>364665132</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="W3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="X3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding test case for add event in calendar section
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05BFA28-FF1C-46BD-9790-B4E22C9E1DFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1AC2A4-2825-42D3-BCCD-2AF46075ED50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
     <sheet name="documents" sheetId="5" r:id="rId5"/>
     <sheet name="company" sheetId="6" r:id="rId6"/>
+    <sheet name="calendar" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
   <si>
     <t>title</t>
   </si>
@@ -550,6 +551,12 @@
   </si>
   <si>
     <t>Pradumna Arts</t>
+  </si>
+  <si>
+    <t>Test title - 1</t>
+  </si>
+  <si>
+    <t>Important</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73F32D-B0D6-4212-BB6D-11E7061AFE47}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1764,4 +1771,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F455BF22-6C45-42EE-A7A3-AC1068FF6988}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test case for validate new form
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1AC2A4-2825-42D3-BCCD-2AF46075ED50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49320C90-AE7C-4879-8FA4-1370DDC8F9D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="documents" sheetId="5" r:id="rId5"/>
     <sheet name="company" sheetId="6" r:id="rId6"/>
     <sheet name="calendar" sheetId="7" r:id="rId7"/>
+    <sheet name="forms" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="190">
   <si>
     <t>title</t>
   </si>
@@ -557,6 +558,45 @@
   </si>
   <si>
     <t>Important</t>
+  </si>
+  <si>
+    <t>reportMail</t>
+  </si>
+  <si>
+    <t>weklcomeMessage</t>
+  </si>
+  <si>
+    <t>confirmationMessage</t>
+  </si>
+  <si>
+    <t>Form title  - 1</t>
+  </si>
+  <si>
+    <t>Form title  - 2</t>
+  </si>
+  <si>
+    <t>tejas.niturkar@gmail.com</t>
+  </si>
+  <si>
+    <t>pradumna.arts@gmail.com</t>
+  </si>
+  <si>
+    <t>form description - 1 TEST</t>
+  </si>
+  <si>
+    <t>form description - 2 TEST</t>
+  </si>
+  <si>
+    <t>Test form welcome message - 1</t>
+  </si>
+  <si>
+    <t>Test form welcome message - 2</t>
+  </si>
+  <si>
+    <t>Test form confirmation message - 1</t>
+  </si>
+  <si>
+    <t>Test form confirmation message - 2</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F455BF22-6C45-42EE-A7A3-AC1068FF6988}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1806,4 +1846,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA68599E-2DC1-430F-BDDF-58FA68E882C5}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FA21E6AB-C00C-40A0-B512-0F2B5389ED6F}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FFCD2D81-D617-449D-861F-ECE215B0114E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test case for create new case
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49320C90-AE7C-4879-8FA4-1370DDC8F9D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7F354-C651-4F72-AC9D-1E072215432E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="company" sheetId="6" r:id="rId6"/>
     <sheet name="calendar" sheetId="7" r:id="rId7"/>
     <sheet name="forms" sheetId="8" r:id="rId8"/>
+    <sheet name="case" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="203">
   <si>
     <t>title</t>
   </si>
@@ -597,6 +598,45 @@
   </si>
   <si>
     <t>Test form confirmation message - 2</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Test Case title - 1</t>
+  </si>
+  <si>
+    <t>Enquiring</t>
+  </si>
+  <si>
+    <t>Test identifier - 1</t>
+  </si>
+  <si>
+    <t>Test tags - 1</t>
+  </si>
+  <si>
+    <t>Test description - 1</t>
+  </si>
+  <si>
+    <t>Reviewing</t>
+  </si>
+  <si>
+    <t>Test Case title - 2</t>
+  </si>
+  <si>
+    <t>Test identifier - 2</t>
+  </si>
+  <si>
+    <t>Test tags - 2</t>
+  </si>
+  <si>
+    <t>Test description - 2</t>
+  </si>
+  <si>
+    <t>Complaint</t>
+  </si>
+  <si>
+    <t>General Support</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA68599E-2DC1-430F-BDDF-58FA68E882C5}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1923,4 +1963,97 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C93E2B-3F3D-4064-BEA2-98FA9152DF33}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>